<commit_message>
modifica a file pems template_PEMS_EH05
</commit_message>
<xml_diff>
--- a/data_input.xlsx
+++ b/data_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Commesse\Sviluppo\Alarm_automation_PI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C812233-35C2-4D96-B6A8-8AD242294CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9779F9FE-9DF8-4335-B66E-AE061920D1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB9272F1-67AB-4F1E-9686-A9D81288A326}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:I23"/>
+      <selection activeCell="B3" sqref="B3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -599,7 +599,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
       <c r="L2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -637,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -652,7 +652,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -682,7 +682,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -697,7 +697,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -785,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -800,7 +800,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -815,7 +815,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -830,7 +830,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -845,7 +845,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -875,7 +875,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -890,7 +890,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>

</xml_diff>

<commit_message>
funzionante BBe BR -> testare il resto
</commit_message>
<xml_diff>
--- a/data_input.xlsx
+++ b/data_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Commesse\Sviluppo\Alarm_automation_PI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7A4053-BF67-4107-B132-3CF5D825D17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B177395C-035A-4C35-843E-496BC7E2B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB9272F1-67AB-4F1E-9686-A9D81288A326}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,34 +42,7 @@
     <t>Tipo 1</t>
   </si>
   <si>
-    <t>Tipo 2</t>
-  </si>
-  <si>
-    <t>Tipo 3</t>
-  </si>
-  <si>
-    <t>Tipo 4</t>
-  </si>
-  <si>
-    <t>n BR per BB</t>
-  </si>
-  <si>
     <t>n tot PI</t>
-  </si>
-  <si>
-    <t>EH05HD</t>
-  </si>
-  <si>
-    <t>PH2HD</t>
-  </si>
-  <si>
-    <t>n other inverter</t>
-  </si>
-  <si>
-    <t>spare</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t xml:space="preserve">n tipo </t>
@@ -81,10 +54,37 @@
     <t>n BB per EH</t>
   </si>
   <si>
+    <t>n BR per BB</t>
+  </si>
+  <si>
     <t>n C-BESSHD per PH</t>
   </si>
   <si>
+    <t>n other inverter</t>
+  </si>
+  <si>
+    <t>EH05HD</t>
+  </si>
+  <si>
+    <t>PH2HD</t>
+  </si>
+  <si>
+    <t>spare</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Tipo 2</t>
+  </si>
+  <si>
+    <t>Tipo 3</t>
+  </si>
+  <si>
     <t>PCS</t>
+  </si>
+  <si>
+    <t>Tipo 4</t>
   </si>
   <si>
     <t xml:space="preserve">PI </t>
@@ -94,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,7 +250,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -554,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,10 +565,10 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B23" sqref="B23:I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="6.140625" customWidth="1"/>
@@ -577,7 +577,7 @@
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -590,15 +590,15 @@
       <c r="H1" s="9"/>
       <c r="I1" s="10"/>
       <c r="L1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -608,15 +608,15 @@
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
       <c r="L2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -626,12 +626,12 @@
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -641,12 +641,12 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -656,12 +656,12 @@
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -671,9 +671,9 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -686,12 +686,12 @@
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -701,12 +701,12 @@
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -716,12 +716,12 @@
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -731,12 +731,12 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -746,12 +746,12 @@
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -761,12 +761,12 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -776,9 +776,9 @@
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1">
       <c r="A14" s="8" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -789,12 +789,12 @@
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B15" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -804,12 +804,12 @@
       <c r="H15" s="6"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -819,12 +819,12 @@
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -834,12 +834,12 @@
       <c r="H17" s="2"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -849,12 +849,12 @@
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -864,9 +864,9 @@
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -879,12 +879,12 @@
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -894,12 +894,12 @@
       <c r="H21" s="2"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -909,12 +909,12 @@
       <c r="H22" s="2"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -924,12 +924,12 @@
       <c r="H23" s="2"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -939,12 +939,12 @@
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -954,12 +954,12 @@
       <c r="H25" s="2"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -969,9 +969,9 @@
       <c r="H26" s="4"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1">
       <c r="A27" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -982,9 +982,9 @@
       <c r="H27" s="9"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B28" s="6">
         <v>0</v>
@@ -997,9 +997,9 @@
       <c r="H28" s="6"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
@@ -1012,9 +1012,9 @@
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
@@ -1027,9 +1027,9 @@
       <c r="H30" s="2"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
@@ -1042,9 +1042,9 @@
       <c r="H31" s="2"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
@@ -1057,9 +1057,9 @@
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
@@ -1072,9 +1072,9 @@
       <c r="H33" s="2"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B34" s="2">
         <v>0</v>
@@ -1087,9 +1087,9 @@
       <c r="H34" s="2"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -1102,12 +1102,12 @@
       <c r="H35" s="2"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1117,12 +1117,12 @@
       <c r="H36" s="2"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1132,12 +1132,12 @@
       <c r="H37" s="2"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1147,12 +1147,12 @@
       <c r="H38" s="2"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15.75" thickBot="1">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -1162,9 +1162,9 @@
       <c r="H39" s="4"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15.75" thickBot="1">
       <c r="A40" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1175,9 +1175,9 @@
       <c r="H40" s="9"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B41" s="6">
         <v>0</v>
@@ -1190,9 +1190,9 @@
       <c r="H41" s="6"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B42" s="2">
         <v>0</v>
@@ -1205,9 +1205,9 @@
       <c r="H42" s="2"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B43" s="2">
         <v>0</v>
@@ -1220,9 +1220,9 @@
       <c r="H43" s="2"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B44" s="2">
         <v>0</v>
@@ -1235,9 +1235,9 @@
       <c r="H44" s="2"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B45" s="2">
         <v>0</v>
@@ -1250,9 +1250,9 @@
       <c r="H45" s="2"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" s="2">
         <v>0</v>
@@ -1265,9 +1265,9 @@
       <c r="H46" s="2"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B47" s="2">
         <v>0</v>
@@ -1280,9 +1280,9 @@
       <c r="H47" s="2"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B48" s="2">
         <v>0</v>
@@ -1295,12 +1295,12 @@
       <c r="H48" s="2"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1310,12 +1310,12 @@
       <c r="H49" s="2"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1325,12 +1325,12 @@
       <c r="H50" s="2"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1340,12 +1340,12 @@
       <c r="H51" s="2"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15.75" thickBot="1">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -1423,12 +1423,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1436,4 +1436,286 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100260B53F379FC324F8380158707F79306" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1cc1db398b3b42028473d294ab7d7c2a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="013edbdd-9b27-46fe-aec1-397647bd8b02" xmlns:ns3="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c26e9d514a351cad79ec610caaceaf8" ns2:_="" ns3:_="">
+    <xsd:import namespace="013edbdd-9b27-46fe-aec1-397647bd8b02"/>
+    <xsd:import namespace="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:b1b820adfd3e4a078472514c1a5cb5ff" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="013edbdd-9b27-46fe-aec1-397647bd8b02" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="b1b820adfd3e4a078472514c1a5cb5ff" ma:index="6" nillable="true" ma:displayName="Security Classification_0" ma:hidden="true" ma:internalName="b1b820adfd3e4a078472514c1a5cb5ff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="7" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{06fb96f4-38bd-4123-94b2-8c5938bb75db}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="013edbdd-9b27-46fe-aec1-397647bd8b02">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:SearchPeopleOnly="false" ma:SharePointGroup="0" ma:internalName="SharedWithUsers" ma:readOnly="true" ma:showField="ImnName">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="22" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="25" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="9f302db3-da21-42b3-bdf2-187d2253b329" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="20" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
+    <b1b820adfd3e4a078472514c1a5cb5ff xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C99B41C8-3253-4B72-9933-4F831850EA71}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87397DAA-F3C0-490F-9334-B39E2C617ADE}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EC6A27B-61C6-4574-B215-AE411A3C44AD}"/>
 </file>
</xml_diff>